<commit_message>
update to consumer problem
</commit_message>
<xml_diff>
--- a/Model Writeup/Notation_Guide.xlsx
+++ b/Model Writeup/Notation_Guide.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="EndogenousVariables" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="323">
   <si>
     <t>Variable</t>
   </si>
@@ -975,6 +975,21 @@
   </si>
   <si>
     <t xml:space="preserve"> firm of sector $C$ and industry $m$ at time $t$</t>
+  </si>
+  <si>
+    <t>\ \ \ $\tilde{c}_{j,s,t}$</t>
+  </si>
+  <si>
+    <t>$c_{j,s,t}=\tilde{c}_{j,s,t}+ \sum_{i}^{I}\bar{c}_{i,j,s,t}$</t>
+  </si>
+  <si>
+    <t>Discretionary consumption of composite consumption good by household of lifetime income group $j$, age $s$, at time $t$</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> \ \ \ $c_{i,j,s,t}$</t>
+  </si>
+  <si>
+    <t>Consumption of consumption good $i$ by household of lifetime income group $j$, age $s$, at time $t$</t>
   </si>
 </sst>
 </file>
@@ -1030,8 +1045,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="157">
+  <cellStyleXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1193,7 +1210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="157">
+  <cellStyles count="159">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1272,6 +1289,7 @@
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1350,6 +1368,7 @@
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1679,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1719,441 +1738,460 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>268</v>
+        <v>318</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>270</v>
+        <v>321</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>322</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="B9" t="s">
-        <v>266</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>273</v>
-      </c>
-      <c r="B12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
+        <v>264</v>
+      </c>
+      <c r="B11" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>274</v>
-      </c>
-      <c r="B13" t="s">
-        <v>209</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>275</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>210</v>
+        <v>273</v>
+      </c>
+      <c r="B14" t="s">
+        <v>208</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>277</v>
-      </c>
-      <c r="B16" t="s">
-        <v>314</v>
+        <v>275</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>276</v>
+      </c>
       <c r="B17" t="s">
-        <v>315</v>
+        <v>211</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B18" t="s">
-        <v>212</v>
+        <v>314</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>279</v>
-      </c>
       <c r="B19" t="s">
-        <v>213</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>14</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B20" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B25" t="s">
-        <v>316</v>
+        <v>217</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>284</v>
+      </c>
       <c r="B26" t="s">
-        <v>317</v>
+        <v>218</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
+        <v>285</v>
+      </c>
+      <c r="B27" t="s">
+        <v>316</v>
+      </c>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
         <v>286</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>219</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>38</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D29" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>287</v>
-      </c>
-      <c r="B28" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>288</v>
-      </c>
-      <c r="B31" t="s">
-        <v>185</v>
+        <v>287</v>
+      </c>
+      <c r="B30" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>289</v>
-      </c>
-      <c r="B32" t="s">
-        <v>186</v>
-      </c>
-      <c r="C32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B33" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B34" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+      <c r="C34" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B36" t="s">
-        <v>191</v>
-      </c>
-      <c r="D36" t="s">
-        <v>192</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>292</v>
+      </c>
+      <c r="B37" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" t="s">
-        <v>294</v>
-      </c>
-      <c r="B39" t="s">
-        <v>161</v>
-      </c>
-      <c r="D39" t="s">
-        <v>164</v>
-      </c>
-      <c r="E39" t="s">
-        <v>163</v>
+        <v>293</v>
+      </c>
+      <c r="B38" t="s">
+        <v>191</v>
+      </c>
+      <c r="D38" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>295</v>
-      </c>
-      <c r="B40" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B41" t="s">
-        <v>183</v>
+        <v>161</v>
+      </c>
+      <c r="D41" t="s">
+        <v>164</v>
+      </c>
+      <c r="E41" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B42" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B43" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B44" t="s">
-        <v>265</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B45" t="s">
-        <v>301</v>
+        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B46" t="s">
-        <v>303</v>
+        <v>265</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B47" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B48" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B49" t="s">
-        <v>309</v>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>306</v>
+      </c>
+      <c r="B50" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
-        <v>194</v>
+        <v>308</v>
+      </c>
+      <c r="B51" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2279,8 +2317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B75" sqref="A1:B75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updates to notation guide
</commit_message>
<xml_diff>
--- a/Model Writeup/Notation_Guide.xlsx
+++ b/Model Writeup/Notation_Guide.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="EndogenousVariables" sheetId="4" r:id="rId1"/>
     <sheet name="ExogenousVariables" sheetId="5" r:id="rId2"/>
     <sheet name="Parameters" sheetId="3" r:id="rId3"/>
+    <sheet name="Rules and letters used" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="539">
   <si>
     <t>Variable</t>
   </si>
@@ -296,9 +297,6 @@
     <t>Set based on population in base year</t>
   </si>
   <si>
-    <t>\ \ \ $w_{s,0}$</t>
-  </si>
-  <si>
     <t>\ \ \ $J$</t>
   </si>
   <si>
@@ -530,9 +528,6 @@
     <t>``Transition" matrix relating output of firms to the supply of new capital (dimesions are $M\times M$)</t>
   </si>
   <si>
-    <t>``Transition" matrix relating output of firms to consumption goods (dimesions are $M\times I$)</t>
-  </si>
-  <si>
     <t>Share parameter for corporate output in industry $m$</t>
   </si>
   <si>
@@ -990,13 +985,667 @@
   </si>
   <si>
     <t>Consumption of consumption good $i$ by household of lifetime income group $j$, age $s$, at time $t$</t>
+  </si>
+  <si>
+    <t>Rules:</t>
+  </si>
+  <si>
+    <t>1) Use tilde for stationarized versions of variables</t>
+  </si>
+  <si>
+    <t>2) Use hats for percent deviations from steady state (or percent changes?)</t>
+  </si>
+  <si>
+    <t>English Alphabet</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Letter</t>
+  </si>
+  <si>
+    <t>4) English alphabet for variables, greek for parameters</t>
+  </si>
+  <si>
+    <t>taxable income - labor plus capital income</t>
+  </si>
+  <si>
+    <t>consumption</t>
+  </si>
+  <si>
+    <t>effective labor units</t>
+  </si>
+  <si>
+    <t>wage rate</t>
+  </si>
+  <si>
+    <t>labor supply</t>
+  </si>
+  <si>
+    <t>labor endowment</t>
+  </si>
+  <si>
+    <t>real interest rate</t>
+  </si>
+  <si>
+    <t>prices</t>
+  </si>
+  <si>
+    <t>denotes age</t>
+  </si>
+  <si>
+    <t>denotes calendar year</t>
+  </si>
+  <si>
+    <t>denotes production industry</t>
+  </si>
+  <si>
+    <t>denotes lifetime income group</t>
+  </si>
+  <si>
+    <t>denotes consumption good category, denotes immigration rate</t>
+  </si>
+  <si>
+    <t>Working age population</t>
+  </si>
+  <si>
+    <t>Greek Alphabet</t>
+  </si>
+  <si>
+    <t>$\alpha$</t>
+  </si>
+  <si>
+    <t>$\beta$</t>
+  </si>
+  <si>
+    <t>$\gamma$</t>
+  </si>
+  <si>
+    <t>$\delta$</t>
+  </si>
+  <si>
+    <t>$\varepsilon$</t>
+  </si>
+  <si>
+    <t>$\zeta$</t>
+  </si>
+  <si>
+    <t>$\eta$</t>
+  </si>
+  <si>
+    <t>$\theta$</t>
+  </si>
+  <si>
+    <t>$\iota$</t>
+  </si>
+  <si>
+    <t>$\kappa$</t>
+  </si>
+  <si>
+    <t>$\lambda$</t>
+  </si>
+  <si>
+    <t>$\mu$</t>
+  </si>
+  <si>
+    <t>$\nu$</t>
+  </si>
+  <si>
+    <t>$\xi$</t>
+  </si>
+  <si>
+    <t>$\omicron$</t>
+  </si>
+  <si>
+    <t>$\pi$</t>
+  </si>
+  <si>
+    <t>$\rho$</t>
+  </si>
+  <si>
+    <t>$\sigma$</t>
+  </si>
+  <si>
+    <t>$\tau$</t>
+  </si>
+  <si>
+    <t>$\upsilon$</t>
+  </si>
+  <si>
+    <t>$\phi$</t>
+  </si>
+  <si>
+    <t>$\chi$</t>
+  </si>
+  <si>
+    <t>$\psi$</t>
+  </si>
+  <si>
+    <t>$\omega$</t>
+  </si>
+  <si>
+    <t>$\Alpha$</t>
+  </si>
+  <si>
+    <t>$\Beta$</t>
+  </si>
+  <si>
+    <t>$\Gamma$</t>
+  </si>
+  <si>
+    <t>$\Delta$</t>
+  </si>
+  <si>
+    <t>$\Epsilon$</t>
+  </si>
+  <si>
+    <t>$\Zeta$</t>
+  </si>
+  <si>
+    <t>$\Eta$</t>
+  </si>
+  <si>
+    <t>$\Theta$</t>
+  </si>
+  <si>
+    <t>$\Iota$</t>
+  </si>
+  <si>
+    <t>$\Kappa$</t>
+  </si>
+  <si>
+    <t>$\Lambda$</t>
+  </si>
+  <si>
+    <t>$\Mu$</t>
+  </si>
+  <si>
+    <t>$\Nu$</t>
+  </si>
+  <si>
+    <t>$\Xi$</t>
+  </si>
+  <si>
+    <t>$\Omicron$</t>
+  </si>
+  <si>
+    <t>$\Pi$</t>
+  </si>
+  <si>
+    <t>$\Rho$</t>
+  </si>
+  <si>
+    <t>$\Sigma$</t>
+  </si>
+  <si>
+    <t>$\Tau$</t>
+  </si>
+  <si>
+    <t>$\Upsilon$</t>
+  </si>
+  <si>
+    <t>$\Phi$</t>
+  </si>
+  <si>
+    <t>$\Chi$</t>
+  </si>
+  <si>
+    <t>$\Psi$</t>
+  </si>
+  <si>
+    <t>$\Omega$</t>
+  </si>
+  <si>
+    <t>Matrix to bridge production to consumption goods</t>
+  </si>
+  <si>
+    <t>Production output</t>
+  </si>
+  <si>
+    <t>Number of production sectors</t>
+  </si>
+  <si>
+    <t>Number of lifetime income groups</t>
+  </si>
+  <si>
+    <t>elements of Z</t>
+  </si>
+  <si>
+    <t>Capital stock</t>
+  </si>
+  <si>
+    <t>denotes years ahead in sequence problem, utility function</t>
+  </si>
+  <si>
+    <t>Invetsment adjustment costs born by the firms</t>
+  </si>
+  <si>
+    <t>Firm value</t>
+  </si>
+  <si>
+    <t>Average Q</t>
+  </si>
+  <si>
+    <t>Tobin's marginal q</t>
+  </si>
+  <si>
+    <t>Government spending</t>
+  </si>
+  <si>
+    <t>Total economic output</t>
+  </si>
+  <si>
+    <t>Number of consumption goods, investment by firms and government</t>
+  </si>
+  <si>
+    <t>Number of years to SS (guess for TPI method), Total taxes, Transfers</t>
+  </si>
+  <si>
+    <t>Distribution of assets</t>
+  </si>
+  <si>
+    <t>Beliefs about eq'm path of prices, Matrix relating production goods to capital stock</t>
+  </si>
+  <si>
+    <t>Measure of households of a given type</t>
+  </si>
+  <si>
+    <t>\ \ \ $\omega_{s,0}$</t>
+  </si>
+  <si>
+    <t>Coeff of relative risk aversion</t>
+  </si>
+  <si>
+    <t>Marginal tax rates</t>
+  </si>
+  <si>
+    <t>Utility weights for disutility of labor, utility of bequests</t>
+  </si>
+  <si>
+    <t>Consumption share parameter</t>
+  </si>
+  <si>
+    <t>Depreciation rates</t>
+  </si>
+  <si>
+    <t>Fraction of population of each lifetime income group</t>
+  </si>
+  <si>
+    <t>shift parameter in disutility of labor function</t>
+  </si>
+  <si>
+    <t>Frisch elasticity of labor supply</t>
+  </si>
+  <si>
+    <t>Age at which retirement benefits are paid out</t>
+  </si>
+  <si>
+    <t>Debt held by firm, Aggregate household assets, Coefficient on the linear term in the individual income tax function</t>
+  </si>
+  <si>
+    <t>Government Debt, Level parameter in the individual income tax function</t>
+  </si>
+  <si>
+    <t>Social security system replacement rate</t>
+  </si>
+  <si>
+    <t>CES weights for corp vs noncorp output,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elasticity in CES production function, Elasticity in CES preferences over corp/non corp output </t>
+  </si>
+  <si>
+    <t>Household rate of time preference, Scaling parameters in firm investment adjustment costs</t>
+  </si>
+  <si>
+    <t>Steady state investment rate by firms</t>
+  </si>
+  <si>
+    <t>asset holdings of household, scale parameter in disutility of labor function, debt to capital ratio parameter for firms</t>
+  </si>
+  <si>
+    <t>fertility rate, dummy variables for firm taxes</t>
+  </si>
+  <si>
+    <t>Mortality rate, response rate for gov't spending as a function of debt</t>
+  </si>
+  <si>
+    <t>population growth rate, growth rate in labor augmenting tech</t>
+  </si>
+  <si>
+    <t>Those using multiple letters:</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>Letters</t>
+  </si>
+  <si>
+    <t>Effective labor demand by firms</t>
+  </si>
+  <si>
+    <t>EARN</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>VN</t>
+  </si>
+  <si>
+    <t>New equity issues by firms</t>
+  </si>
+  <si>
+    <t>Total entity level income taxes by firms</t>
+  </si>
+  <si>
+    <t>Dividents distributed by firms</t>
+  </si>
+  <si>
+    <t>Earnings by firms</t>
+  </si>
+  <si>
+    <t>BQ</t>
+  </si>
+  <si>
+    <t>Aggregate bequests</t>
+  </si>
+  <si>
+    <t>Possible Changes:</t>
+  </si>
+  <si>
+    <t>Dividend payout ratio for corporate firms</t>
+  </si>
+  <si>
+    <t>Variable/Parameter</t>
+  </si>
+  <si>
+    <t>Dividends</t>
+  </si>
+  <si>
+    <t>Effective labor demand by firm</t>
+  </si>
+  <si>
+    <t>Firm earnings</t>
+  </si>
+  <si>
+    <t>Firm ouput</t>
+  </si>
+  <si>
+    <t>Use lower case for firm investment, capital stock, output</t>
+  </si>
+  <si>
+    <t>Discounted, expected lifetime utility</t>
+  </si>
+  <si>
+    <t>3) Use capital letters for aggregate values, lower case for per capita values</t>
+  </si>
+  <si>
+    <t>5) Use bars over variable for per capita variables</t>
+  </si>
+  <si>
+    <t>Average Q?? Does break rule for bar used for per capital variables…</t>
+  </si>
+  <si>
+    <t>c_{I,j,s,t} = consumption of good i</t>
+  </si>
+  <si>
+    <t>\tilde{c}_{j,s,t} = discretionary consumption</t>
+  </si>
+  <si>
+    <t>Need to get rid of bars and tildes</t>
+  </si>
+  <si>
+    <t>Issues with consumption:</t>
+  </si>
+  <si>
+    <t>New equity issues?  Does conflict with age, but is used by others (and s=shares)…</t>
+  </si>
+  <si>
+    <t>Aggregate bequests??  Doesn't fit right, but would avoid two letters…</t>
+  </si>
+  <si>
+    <t>How about:</t>
+  </si>
+  <si>
+    <t>``Transition" matrix relating output of firms to consumption goods (dimensions are $M\times I$)</t>
+  </si>
+  <si>
+    <t>c_{j,s,t} = composite consumption for age t = \tilde{c}_{j,s,t} + \bar{c}_{s,t}</t>
+  </si>
+  <si>
+    <t>c = total consumption- either for composite or individual goods</t>
+  </si>
+  <si>
+    <t>gothic c = discretionary consumption of composite good</t>
+  </si>
+  <si>
+    <t>WHAT to use for minimum consumption share???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$\upsilon$ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replace v as labor supply elasticity </t>
+  </si>
+  <si>
+    <t>Use this instread of $Z$ for ``transition" between productions output and consumption goods</t>
+  </si>
+  <si>
+    <t>Use this instread of $\Omega$ for ``transition" between productions output and investment goods/capital</t>
+  </si>
+  <si>
+    <t>Use this instead of $\rho$ for gov't spending response to debt</t>
+  </si>
+  <si>
+    <t>Use this instead of $\lambda$ for lifetime income distribution (saving $\lambda$ for Lagrangian multipliers)</t>
+  </si>
+  <si>
+    <t>$Z$</t>
+  </si>
+  <si>
+    <t>Shift parameter in disutility of labor</t>
+  </si>
+  <si>
+    <t>$d$</t>
+  </si>
+  <si>
+    <t>$l^{d}$</t>
+  </si>
+  <si>
+    <t>$x$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$y$ </t>
+  </si>
+  <si>
+    <t>$T$</t>
+  </si>
+  <si>
+    <t>Total entity level income taxes paid by firm (careful of conflict with indiv taxes)</t>
+  </si>
+  <si>
+    <t>$s$</t>
+  </si>
+  <si>
+    <t>$\bar{q}$</t>
+  </si>
+  <si>
+    <t>$\psi_{1}-\psi_{4}$</t>
+  </si>
+  <si>
+    <t>Parameters of the income tax function</t>
+  </si>
+  <si>
+    <t>Use instead of $\beta$ as scaling parameter in investment adjustment cost function</t>
+  </si>
+  <si>
+    <t>Use instead of $\nu$ as dampening parameter for TPI method</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1027,13 +1676,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1045,7 +1720,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1205,12 +1880,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="177">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1290,6 +1987,15 @@
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1369,6 +2075,15 @@
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1700,7 +2415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1720,100 +2435,100 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B4" t="s">
         <v>318</v>
-      </c>
-      <c r="B4" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>262</v>
+      </c>
+      <c r="B11" t="s">
         <v>264</v>
-      </c>
-      <c r="B11" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -1824,10 +2539,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -1838,10 +2553,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1852,10 +2567,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B17" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
@@ -1866,10 +2581,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B18" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C18" t="s">
         <v>29</v>
@@ -1880,15 +2595,15 @@
     </row>
     <row r="19" spans="1:4">
       <c r="B19" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C20" t="s">
         <v>30</v>
@@ -1899,10 +2614,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B21" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>
@@ -1913,10 +2628,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B22" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
@@ -1927,10 +2642,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
@@ -1941,10 +2656,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B24" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C24" t="s">
         <v>35</v>
@@ -1955,10 +2670,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B25" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C25" t="s">
         <v>36</v>
@@ -1969,10 +2684,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
@@ -1983,10 +2698,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C27" t="s">
         <v>39</v>
@@ -1997,15 +2712,15 @@
     </row>
     <row r="28" spans="1:4">
       <c r="B28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B29" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
@@ -2016,183 +2731,183 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B30" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B33" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B34" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C34" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B35" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B36" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B37" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B38" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D38" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B43" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B44" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B45" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B46" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B47" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B48" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B49" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B50" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B51" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2211,7 +2926,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:B11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2226,39 +2941,39 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" t="s">
         <v>111</v>
-      </c>
-      <c r="E5" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2266,7 +2981,7 @@
         <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D8" t="s">
         <v>90</v>
@@ -2274,10 +2989,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>460</v>
       </c>
       <c r="B9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D9" t="s">
         <v>90</v>
@@ -2285,21 +3000,21 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" t="s">
         <v>197</v>
-      </c>
-      <c r="B10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D10" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2317,8 +3032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2338,23 +3053,23 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
         <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2362,7 +3077,7 @@
         <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
         <v>73</v>
@@ -2376,7 +3091,7 @@
         <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
         <v>76</v>
@@ -2390,7 +3105,7 @@
         <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s">
         <v>78</v>
@@ -2401,16 +3116,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C7">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -2418,16 +3133,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" t="s">
         <v>152</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" t="s">
         <v>153</v>
-      </c>
-      <c r="C8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" t="s">
-        <v>154</v>
       </c>
       <c r="F8">
         <f>17*80</f>
@@ -2436,16 +3151,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" t="s">
         <v>156</v>
       </c>
-      <c r="B9" t="s">
-        <v>157</v>
-      </c>
       <c r="C9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F9">
         <f>17*80</f>
@@ -2454,13 +3169,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>514</v>
       </c>
       <c r="D10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F10">
         <f>24*17</f>
@@ -2469,13 +3184,13 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F11">
         <v>24</v>
@@ -2483,13 +3198,13 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -2497,21 +3212,21 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" t="s">
         <v>172</v>
-      </c>
-      <c r="B14" t="s">
-        <v>177</v>
-      </c>
-      <c r="C14" t="s">
-        <v>175</v>
-      </c>
-      <c r="D14" t="s">
-        <v>174</v>
       </c>
       <c r="F14">
         <f>7*80</f>
@@ -2520,13 +3235,13 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -2534,13 +3249,13 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" t="s">
+        <v>176</v>
+      </c>
+      <c r="D16" t="s">
         <v>93</v>
-      </c>
-      <c r="B16" t="s">
-        <v>178</v>
-      </c>
-      <c r="D16" t="s">
-        <v>94</v>
       </c>
       <c r="F16">
         <v>7</v>
@@ -2551,7 +3266,7 @@
         <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F17">
         <v>80</v>
@@ -2559,10 +3274,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -2570,10 +3285,10 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -2581,10 +3296,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B20" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -2592,13 +3307,13 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" t="s">
         <v>95</v>
-      </c>
-      <c r="B21" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" t="s">
-        <v>96</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -2606,7 +3321,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2614,7 +3329,7 @@
         <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D23" t="s">
         <v>80</v>
@@ -2628,7 +3343,7 @@
         <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" t="s">
         <v>82</v>
@@ -2639,13 +3354,13 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
+        <v>219</v>
+      </c>
+      <c r="B25" t="s">
+        <v>220</v>
+      </c>
+      <c r="D25" t="s">
         <v>221</v>
-      </c>
-      <c r="B25" t="s">
-        <v>222</v>
-      </c>
-      <c r="D25" t="s">
-        <v>223</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -2656,7 +3371,7 @@
         <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
         <v>84</v>
@@ -2670,7 +3385,7 @@
         <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D27" t="s">
         <v>86</v>
@@ -2684,7 +3399,7 @@
         <v>87</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D28" t="s">
         <v>88</v>
@@ -2695,18 +3410,18 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B31" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C31" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -2714,13 +3429,13 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B32" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2728,13 +3443,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B33" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -2742,13 +3457,13 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B34" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C34" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -2756,13 +3471,13 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B35" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C35" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2770,13 +3485,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B36" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C36" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2784,13 +3499,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B37" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C37" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F37">
         <v>7</v>
@@ -2798,13 +3513,13 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C38" t="s">
         <v>238</v>
-      </c>
-      <c r="C38" t="s">
-        <v>240</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -2812,12 +3527,12 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2825,7 +3540,7 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C42" t="s">
         <v>45</v>
@@ -2843,7 +3558,7 @@
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C43" t="s">
         <v>48</v>
@@ -2858,7 +3573,7 @@
         <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C44" t="s">
         <v>50</v>
@@ -2876,7 +3591,7 @@
         <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C45" t="s">
         <v>48</v>
@@ -2891,7 +3606,7 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C46" t="s">
         <v>54</v>
@@ -2903,7 +3618,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2911,7 +3626,7 @@
         <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E48" t="s">
         <v>59</v>
@@ -2925,7 +3640,7 @@
         <v>60</v>
       </c>
       <c r="B49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C49" t="s">
         <v>61</v>
@@ -2939,15 +3654,15 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C51" t="s">
         <v>63</v>
@@ -2958,10 +3673,10 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C52" t="s">
         <v>64</v>
@@ -2975,10 +3690,10 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C53" t="s">
         <v>66</v>
@@ -2989,13 +3704,13 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F54" s="1">
         <v>1</v>
@@ -3003,13 +3718,13 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
@@ -3026,7 +3741,7 @@
         <v>67</v>
       </c>
       <c r="E56" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F56" s="1">
         <v>1</v>
@@ -3034,7 +3749,7 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B57" t="s">
         <v>40</v>
@@ -3043,7 +3758,7 @@
         <v>67</v>
       </c>
       <c r="E57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F57" s="1">
         <v>1</v>
@@ -3060,7 +3775,7 @@
         <v>67</v>
       </c>
       <c r="E58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F58" s="1">
         <v>1</v>
@@ -3077,7 +3792,7 @@
         <v>67</v>
       </c>
       <c r="E59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F59" s="1">
         <v>1</v>
@@ -3094,7 +3809,7 @@
         <v>67</v>
       </c>
       <c r="E60" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F60" s="1">
         <v>1</v>
@@ -3102,12 +3817,12 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B62" t="s">
         <v>70</v>
@@ -3124,16 +3839,16 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D63" t="s">
         <v>71</v>
       </c>
       <c r="E63" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F63">
         <f>24*24</f>
@@ -3142,18 +3857,18 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B66" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C66" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -3166,10 +3881,10 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
+        <v>107</v>
+      </c>
+      <c r="B69" t="s">
         <v>108</v>
-      </c>
-      <c r="B69" t="s">
-        <v>109</v>
       </c>
       <c r="C69" t="s">
         <v>55</v>
@@ -3180,10 +3895,10 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" t="s">
         <v>113</v>
-      </c>
-      <c r="B70" t="s">
-        <v>114</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -3194,7 +3909,7 @@
         <v>56</v>
       </c>
       <c r="B71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C71" t="s">
         <v>57</v>
@@ -3205,18 +3920,18 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B74" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C74" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -3224,13 +3939,13 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B75" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C75" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -3238,11 +3953,888 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F78">
-        <f>SUM(F42:F75)</f>
-        <v>1046</v>
+        <f>SUM(F4:F75)</f>
+        <v>5112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>324</v>
+      </c>
+      <c r="H7" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>377</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>377</v>
+      </c>
+      <c r="I8" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>377</v>
+      </c>
+      <c r="M8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>325</v>
+      </c>
+      <c r="B9" t="s">
+        <v>379</v>
+      </c>
+      <c r="D9" t="s">
+        <v>351</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="H9" t="s">
+        <v>394</v>
+      </c>
+      <c r="I9" t="s">
+        <v>464</v>
+      </c>
+      <c r="L9" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="L10" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>327</v>
+      </c>
+      <c r="B11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D11" t="s">
+        <v>353</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H11" t="s">
+        <v>396</v>
+      </c>
+      <c r="I11" t="s">
+        <v>473</v>
+      </c>
+      <c r="L11" t="s">
+        <v>420</v>
+      </c>
+      <c r="M11" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>328</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="H12" t="s">
+        <v>397</v>
+      </c>
+      <c r="I12" t="s">
+        <v>465</v>
+      </c>
+      <c r="L12" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13" t="s">
+        <v>381</v>
+      </c>
+      <c r="D13" t="s">
+        <v>355</v>
+      </c>
+      <c r="E13" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" t="s">
+        <v>398</v>
+      </c>
+      <c r="I13" t="s">
+        <v>474</v>
+      </c>
+      <c r="L13" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="D14" t="s">
+        <v>356</v>
+      </c>
+      <c r="E14" t="s">
+        <v>230</v>
+      </c>
+      <c r="H14" t="s">
+        <v>399</v>
+      </c>
+      <c r="I14" t="s">
+        <v>496</v>
+      </c>
+      <c r="L14" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" t="s">
+        <v>480</v>
+      </c>
+      <c r="D15" t="s">
+        <v>357</v>
+      </c>
+      <c r="E15" t="s">
+        <v>453</v>
+      </c>
+      <c r="H15" t="s">
+        <v>400</v>
+      </c>
+      <c r="L15" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>332</v>
+      </c>
+      <c r="D16" t="s">
+        <v>358</v>
+      </c>
+      <c r="H16" t="s">
+        <v>401</v>
+      </c>
+      <c r="I16" t="s">
+        <v>472</v>
+      </c>
+      <c r="L16" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D17" t="s">
+        <v>359</v>
+      </c>
+      <c r="E17" t="s">
+        <v>455</v>
+      </c>
+      <c r="H17" t="s">
+        <v>402</v>
+      </c>
+      <c r="L17" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>334</v>
+      </c>
+      <c r="B18" t="s">
+        <v>390</v>
+      </c>
+      <c r="D18" t="s">
+        <v>360</v>
+      </c>
+      <c r="E18" t="s">
+        <v>445</v>
+      </c>
+      <c r="H18" t="s">
+        <v>403</v>
+      </c>
+      <c r="L18" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>335</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="L19" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>336</v>
+      </c>
+      <c r="B20" t="s">
+        <v>384</v>
+      </c>
+      <c r="D20" t="s">
+        <v>362</v>
+      </c>
+      <c r="H20" t="s">
+        <v>405</v>
+      </c>
+      <c r="I20" t="s">
+        <v>476</v>
+      </c>
+      <c r="L20" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>337</v>
+      </c>
+      <c r="B21" t="s">
+        <v>389</v>
+      </c>
+      <c r="D21" t="s">
+        <v>363</v>
+      </c>
+      <c r="E21" t="s">
+        <v>444</v>
+      </c>
+      <c r="H21" t="s">
+        <v>406</v>
+      </c>
+      <c r="I21" t="s">
+        <v>232</v>
+      </c>
+      <c r="L21" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>338</v>
+      </c>
+      <c r="B22" t="s">
+        <v>383</v>
+      </c>
+      <c r="D22" t="s">
+        <v>364</v>
+      </c>
+      <c r="E22" t="s">
+        <v>392</v>
+      </c>
+      <c r="H22" t="s">
+        <v>407</v>
+      </c>
+      <c r="L22" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>339</v>
+      </c>
+      <c r="D23" t="s">
+        <v>365</v>
+      </c>
+      <c r="H23" t="s">
+        <v>408</v>
+      </c>
+      <c r="L23" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>340</v>
+      </c>
+      <c r="B24" t="s">
+        <v>386</v>
+      </c>
+      <c r="D24" t="s">
+        <v>366</v>
+      </c>
+      <c r="H24" t="s">
+        <v>409</v>
+      </c>
+      <c r="L24" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>341</v>
+      </c>
+      <c r="B25" t="s">
+        <v>452</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="H25" t="s">
+        <v>410</v>
+      </c>
+      <c r="I25" t="s">
+        <v>479</v>
+      </c>
+      <c r="L25" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>342</v>
+      </c>
+      <c r="B26" t="s">
+        <v>385</v>
+      </c>
+      <c r="D26" t="s">
+        <v>368</v>
+      </c>
+      <c r="E26" t="s">
+        <v>469</v>
+      </c>
+      <c r="H26" t="s">
+        <v>411</v>
+      </c>
+      <c r="I26" t="s">
+        <v>461</v>
+      </c>
+      <c r="L26" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B27" t="s">
+        <v>387</v>
+      </c>
+      <c r="D27" t="s">
+        <v>369</v>
+      </c>
+      <c r="E27" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" t="s">
+        <v>412</v>
+      </c>
+      <c r="I27" t="s">
+        <v>462</v>
+      </c>
+      <c r="L27" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>344</v>
+      </c>
+      <c r="B28" t="s">
+        <v>388</v>
+      </c>
+      <c r="D28" t="s">
+        <v>370</v>
+      </c>
+      <c r="E28" t="s">
+        <v>456</v>
+      </c>
+      <c r="H28" t="s">
+        <v>413</v>
+      </c>
+      <c r="L28" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" t="s">
+        <v>345</v>
+      </c>
+      <c r="B29" t="s">
+        <v>448</v>
+      </c>
+      <c r="D29" t="s">
+        <v>371</v>
+      </c>
+      <c r="E29" t="s">
+        <v>503</v>
+      </c>
+      <c r="H29" t="s">
+        <v>414</v>
+      </c>
+      <c r="L29" t="s">
+        <v>438</v>
+      </c>
+      <c r="M29" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" t="s">
+        <v>346</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="D30" t="s">
+        <v>372</v>
+      </c>
+      <c r="E30" t="s">
+        <v>450</v>
+      </c>
+      <c r="H30" t="s">
+        <v>415</v>
+      </c>
+      <c r="I30" t="s">
+        <v>463</v>
+      </c>
+      <c r="L30" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
+        <v>347</v>
+      </c>
+      <c r="B31" t="s">
+        <v>382</v>
+      </c>
+      <c r="D31" t="s">
+        <v>373</v>
+      </c>
+      <c r="H31" t="s">
+        <v>416</v>
+      </c>
+      <c r="L31" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
+        <v>348</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="H32" t="s">
+        <v>417</v>
+      </c>
+      <c r="I32" t="s">
+        <v>459</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>349</v>
+      </c>
+      <c r="D33" t="s">
+        <v>375</v>
+      </c>
+      <c r="E33" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>350</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="D34" t="s">
+        <v>376</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>483</v>
+      </c>
+      <c r="B38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>482</v>
+      </c>
+      <c r="B39" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>485</v>
+      </c>
+      <c r="B40" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>486</v>
+      </c>
+      <c r="B41" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>487</v>
+      </c>
+      <c r="B42" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>488</v>
+      </c>
+      <c r="B43" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>493</v>
+      </c>
+      <c r="B44" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>377</v>
+      </c>
+      <c r="B49" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>527</v>
+      </c>
+      <c r="B50" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>528</v>
+      </c>
+      <c r="B51" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>529</v>
+      </c>
+      <c r="B52" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>530</v>
+      </c>
+      <c r="B53" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>531</v>
+      </c>
+      <c r="B54" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>533</v>
+      </c>
+      <c r="B55" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>519</v>
+      </c>
+      <c r="B56" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>534</v>
+      </c>
+      <c r="B57" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>433</v>
+      </c>
+      <c r="B58" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>431</v>
+      </c>
+      <c r="B59" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>414</v>
+      </c>
+      <c r="B60" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>400</v>
+      </c>
+      <c r="B61" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>525</v>
+      </c>
+      <c r="B62" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>403</v>
+      </c>
+      <c r="B63" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>535</v>
+      </c>
+      <c r="B64" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>406</v>
+      </c>
+      <c r="B65" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>421</v>
+      </c>
+      <c r="B66" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="5" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edits to firm problem and notation
</commit_message>
<xml_diff>
--- a/Model Writeup/Notation_Guide.xlsx
+++ b/Model Writeup/Notation_Guide.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="EndogenousVariables" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="541">
   <si>
     <t>Variable</t>
   </si>
@@ -495,9 +495,6 @@
     <t>Household sub-utility function minimum amount of good $i$ for households of age $s$</t>
   </si>
   <si>
-    <t>Price of composite consumption good for household of age $s$</t>
-  </si>
-  <si>
     <t>Price of consumption good $i$ at time $t$</t>
   </si>
   <si>
@@ -831,9 +828,6 @@
     <t>\ \ \ $b_{j,s,t}$</t>
   </si>
   <si>
-    <t>\ \ \ $p_{s,t}$</t>
-  </si>
-  <si>
     <t>\ \ \ $p_{i,t}$</t>
   </si>
   <si>
@@ -990,12 +984,6 @@
     <t>Rules:</t>
   </si>
   <si>
-    <t>1) Use tilde for stationarized versions of variables</t>
-  </si>
-  <si>
-    <t>2) Use hats for percent deviations from steady state (or percent changes?)</t>
-  </si>
-  <si>
     <t>English Alphabet</t>
   </si>
   <si>
@@ -1536,12 +1524,6 @@
     <t>Discounted, expected lifetime utility</t>
   </si>
   <si>
-    <t>3) Use capital letters for aggregate values, lower case for per capita values</t>
-  </si>
-  <si>
-    <t>5) Use bars over variable for per capita variables</t>
-  </si>
-  <si>
     <t>Average Q?? Does break rule for bar used for per capital variables…</t>
   </si>
   <si>
@@ -1639,6 +1621,30 @@
   </si>
   <si>
     <t>Use instead of $\nu$ as dampening parameter for TPI method</t>
+  </si>
+  <si>
+    <t>1) Use hat for stationarized versions of variables</t>
+  </si>
+  <si>
+    <t>5) Use bars over variable for steady state</t>
+  </si>
+  <si>
+    <t>2) Use tilde for special values of variable</t>
+  </si>
+  <si>
+    <t>3) Use capital letters for aggregate values, lower case for per capita values --- ignore</t>
+  </si>
+  <si>
+    <t>\ \ \ $\tilde{p}_{s,t}$</t>
+  </si>
+  <si>
+    <t>Price of discretionary composite consumption good for household of age $s$</t>
+  </si>
+  <si>
+    <t>\ \ \ $p^{K}_{m,C,t}$</t>
+  </si>
+  <si>
+    <t>Price of capital for sector $C$, industry $m$, at time $t$.</t>
   </si>
 </sst>
 </file>
@@ -1720,8 +1726,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="177">
+  <cellStyleXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1907,7 +1915,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="177">
+  <cellStyles count="179">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1996,6 +2004,7 @@
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2084,6 +2093,7 @@
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2413,10 +2423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2435,7 +2445,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2445,7 +2455,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B3" t="s">
         <v>114</v>
@@ -2453,34 +2463,34 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B4" t="s">
         <v>316</v>
-      </c>
-      <c r="B4" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B5" t="s">
         <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B7" t="s">
         <v>117</v>
@@ -2488,7 +2498,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B8" t="s">
         <v>118</v>
@@ -2496,39 +2506,39 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>537</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>538</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
@@ -2539,10 +2549,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -2553,10 +2563,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -2567,10 +2577,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
@@ -2581,10 +2591,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B18" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C18" t="s">
         <v>29</v>
@@ -2595,15 +2605,15 @@
     </row>
     <row r="19" spans="1:4">
       <c r="B19" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C20" t="s">
         <v>30</v>
@@ -2614,10 +2624,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C21" t="s">
         <v>31</v>
@@ -2628,10 +2638,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
@@ -2642,10 +2652,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
@@ -2656,10 +2666,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C24" t="s">
         <v>35</v>
@@ -2670,10 +2680,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C25" t="s">
         <v>36</v>
@@ -2684,10 +2694,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
@@ -2698,10 +2708,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B27" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C27" t="s">
         <v>39</v>
@@ -2712,15 +2722,15 @@
     </row>
     <row r="28" spans="1:4">
       <c r="B28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
@@ -2731,109 +2741,109 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B30" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>182</v>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>539</v>
+      </c>
+      <c r="B31" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>286</v>
-      </c>
-      <c r="B33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B34" t="s">
-        <v>184</v>
-      </c>
-      <c r="C34" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B35" t="s">
-        <v>186</v>
+        <v>183</v>
+      </c>
+      <c r="C35" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B36" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B37" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>289</v>
+      </c>
+      <c r="B39" t="s">
+        <v>188</v>
+      </c>
+      <c r="D39" t="s">
         <v>189</v>
-      </c>
-      <c r="D38" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>292</v>
-      </c>
-      <c r="B41" t="s">
-        <v>160</v>
-      </c>
-      <c r="D41" t="s">
-        <v>163</v>
-      </c>
-      <c r="E41" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B42" t="s">
-        <v>164</v>
+        <v>159</v>
+      </c>
+      <c r="D42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B43" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B44" t="s">
         <v>180</v>
@@ -2841,73 +2851,81 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B45" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B46" t="s">
-        <v>263</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B47" t="s">
-        <v>299</v>
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B48" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B49" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B50" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B51" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>191</v>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>304</v>
+      </c>
+      <c r="B52" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>194</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2946,7 +2964,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B3" t="s">
         <v>100</v>
@@ -2954,7 +2972,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B4" t="s">
         <v>109</v>
@@ -2962,7 +2980,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B5" t="s">
         <v>110</v>
@@ -2973,7 +2991,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2981,7 +2999,7 @@
         <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D8" t="s">
         <v>90</v>
@@ -2989,10 +3007,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D9" t="s">
         <v>90</v>
@@ -3000,21 +3018,21 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" t="s">
         <v>195</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>196</v>
-      </c>
-      <c r="D10" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" t="s">
         <v>222</v>
-      </c>
-      <c r="B11" t="s">
-        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -3059,7 +3077,7 @@
         <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3069,7 +3087,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3119,13 +3137,13 @@
         <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -3172,10 +3190,10 @@
         <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="D10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F10">
         <f>24*17</f>
@@ -3187,7 +3205,7 @@
         <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>97</v>
@@ -3198,10 +3216,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>97</v>
@@ -3212,21 +3230,21 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F14">
         <f>7*80</f>
@@ -3238,10 +3256,10 @@
         <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -3252,7 +3270,7 @@
         <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D16" t="s">
         <v>93</v>
@@ -3274,7 +3292,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B18" t="s">
         <v>124</v>
@@ -3285,7 +3303,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B19" t="s">
         <v>123</v>
@@ -3296,10 +3314,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -3321,7 +3339,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3354,13 +3372,13 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25" t="s">
         <v>219</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>220</v>
-      </c>
-      <c r="D25" t="s">
-        <v>221</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -3410,18 +3428,18 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -3429,13 +3447,13 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -3443,13 +3461,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -3457,13 +3475,13 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -3471,13 +3489,13 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C35" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -3485,13 +3503,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B36" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -3499,13 +3517,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B37" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F37">
         <v>7</v>
@@ -3513,13 +3531,13 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C38" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -3532,7 +3550,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -3618,7 +3636,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3654,7 +3672,7 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3817,12 +3835,12 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B62" t="s">
         <v>70</v>
@@ -3839,10 +3857,10 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B63" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D63" t="s">
         <v>71</v>
@@ -3857,18 +3875,18 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B66" t="s">
+        <v>197</v>
+      </c>
+      <c r="C66" t="s">
         <v>198</v>
-      </c>
-      <c r="C66" t="s">
-        <v>199</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -3920,18 +3938,18 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B74" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C74" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -3939,13 +3957,13 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B75" t="s">
+        <v>231</v>
+      </c>
+      <c r="C75" t="s">
         <v>232</v>
-      </c>
-      <c r="C75" t="s">
-        <v>233</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -3953,7 +3971,7 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F78">
         <f>SUM(F4:F75)</f>
@@ -3975,71 +3993,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>322</v>
+        <v>533</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>323</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>504</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>505</v>
+        <v>534</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="H7" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="I8" t="s">
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="M8" t="s">
         <v>0</v>
@@ -4047,544 +4065,544 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B9" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D9" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H9" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="I9" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="L9" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="L10" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B11" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D11" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H11" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="I11" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="L11" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="M11" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="H12" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="I12" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="L12" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B13" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D13" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E13" t="s">
         <v>103</v>
       </c>
       <c r="H13" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="I13" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="L13" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="D14" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H14" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="I14" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="L14" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B15" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D15" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E15" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="H15" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="L15" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D16" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="H16" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="I16" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="L16" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D17" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E17" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H17" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="L17" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B18" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D18" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E18" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="H18" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="L18" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="L19" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B20" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D20" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H20" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="I20" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="L20" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B21" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D21" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E21" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="H21" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="I21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L21" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B22" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D22" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E22" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="H22" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="L22" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D23" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="H23" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="L23" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B24" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D24" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="H24" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="L24" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B25" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="H25" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="I25" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="L25" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B26" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D26" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E26" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="H26" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="I26" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="L26" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B27" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D27" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E27" t="s">
         <v>102</v>
       </c>
       <c r="H27" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="I27" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="L27" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B28" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D28" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E28" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H28" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="L28" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B29" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D29" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E29" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="H29" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="L29" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="M29" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D30" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E30" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="H30" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="I30" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="L30" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B31" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D31" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H31" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="L31" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="H32" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="I32" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D33" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E33" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D34" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B38" t="s">
         <v>0</v>
@@ -4592,249 +4610,249 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B39" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B40" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B41" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B42" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B43" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="B44" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B49" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="B50" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="B51" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="B52" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="B53" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="B54" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="B55" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="B56" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="B57" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B58" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B59" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B60" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B61" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="B62" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B63" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="B64" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B65" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B66" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="5" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>